<commit_message>
M52 temp sensor inc files
</commit_message>
<xml_diff>
--- a/m52 PnP/M52 temp sensor calibrations.xlsx
+++ b/m52 PnP/M52 temp sensor calibrations.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BF59394-FF1C-489A-B6EB-58FDB6B74224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F4EEE2-5998-4A0F-8A0A-6FE9B68E4269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26520" windowHeight="8445" xr2:uid="{9F799CD1-2A4A-44B5-AD76-2F73834C19F2}"/>
+    <workbookView xWindow="-25560" yWindow="4080" windowWidth="21600" windowHeight="12735" xr2:uid="{9F799CD1-2A4A-44B5-AD76-2F73834C19F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -100,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -116,7 +111,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,7 +410,7 @@
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,10 +489,10 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>5170</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Better temp sensor calibrations
</commit_message>
<xml_diff>
--- a/m52 PnP/M52 temp sensor calibrations.xlsx
+++ b/m52 PnP/M52 temp sensor calibrations.xlsx
@@ -1,53 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F4EEE2-5998-4A0F-8A0A-6FE9B68E4269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DF7117-59F8-48EA-A9B2-0B70CA2DA44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25560" yWindow="4080" windowWidth="21600" windowHeight="12735" xr2:uid="{9F799CD1-2A4A-44B5-AD76-2F73834C19F2}"/>
+    <workbookView xWindow="1890" yWindow="30" windowWidth="27975" windowHeight="15570" xr2:uid="{82CE32EB-BF3E-452E-A707-F10BC49B34FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Temp (C)</t>
+  </si>
+  <si>
+    <t>Resistance (ohm)</t>
+  </si>
+  <si>
+    <t>Values from stock ecus:</t>
+  </si>
+  <si>
+    <t>For speeduino/Megasquirt</t>
+  </si>
+  <si>
+    <t>Bias resistor value (Ohms):</t>
+  </si>
+  <si>
+    <t>Coolant Temp Sensor</t>
+  </si>
+  <si>
+    <t>Temperature °C</t>
+  </si>
   <si>
     <t>Resistance (Ohms)</t>
   </si>
   <si>
-    <t>Bias resistor value (Ohms):</t>
-  </si>
-  <si>
     <t>Intake Air Temp Sensor</t>
   </si>
   <si>
-    <t>Coolant Temp Sensor</t>
-  </si>
-  <si>
-    <t>Temperature °C</t>
+    <t>Intake Air temp sensor</t>
+  </si>
+  <si>
+    <t>Coolant temp sensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,12 +128,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -111,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,101 +448,533 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F106746-37D8-4B33-A5C3-5E76D75A3820}">
-  <dimension ref="B1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E041B05A-DAB4-4FE4-A52A-6BC53413C950}">
+  <dimension ref="C1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="11" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>2490</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="D4" s="1">
+        <v>142.5</v>
+      </c>
+      <c r="E4" s="2">
+        <f>(C4*828)/(5-C4)</f>
+        <v>49.676489294042824</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E19" si="0">(C5*828)/(5-C5)</f>
+        <v>68.297899978350301</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="D6" s="1">
+        <v>110.3</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>115.05239179954442</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <v>99.8</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>153.27518369281819</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="1">
+        <v>-48</v>
+      </c>
+      <c r="I7" s="2">
+        <v>141930.6206896556</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>207.25881470367588</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2826.0158870255959</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>80.3</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>284.60413867239987</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="1">
+        <v>110.3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>115.05239179954442</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>1.621</v>
+      </c>
+      <c r="D10" s="1">
+        <v>69.8</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>397.21456052086421</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>2.0209999999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>561.7280966767371</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>2.964</v>
+      </c>
+      <c r="D12" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>1205.3988212180745</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>3.867</v>
+      </c>
+      <c r="D13" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>2826.0158870255959</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="1">
+        <v>-48</v>
+      </c>
+      <c r="I13" s="2">
+        <v>363686.47058823734</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>4.2240000000000002</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>4507.0515463917536</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4024.9136577708005</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>4.4969999999999999</v>
+      </c>
+      <c r="D15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>7402.616302186877</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="1">
+        <v>110.3</v>
+      </c>
+      <c r="I15" s="2">
+        <v>257.73780622379167</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>12398.837060702886</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>4.819</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-20.3</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>22044.928176795573</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>4.8970000000000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>39366.174757281646</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>4.9710000000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-48</v>
+      </c>
+      <c r="E19" s="2">
+        <f>(C19*828)/(5-C19)</f>
+        <v>141930.6206896556</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>100</v>
-      </c>
-      <c r="C7" s="1">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>0.215</v>
+      </c>
+      <c r="D23" s="1">
+        <v>142.5</v>
+      </c>
+      <c r="E23" s="2">
+        <f>(C23*2490)/(5-C23)</f>
+        <v>111.88087774294671</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="D24" s="1">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24:E38" si="1">(C24*2490)/(5-C24)</f>
+        <v>144.36309775708847</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D25" s="1">
+        <v>110.3</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>257.73780622379167</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="D26" s="1">
+        <v>99.8</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>343.40919435593992</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D27" s="1">
+        <v>90</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>461.63584637268849</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>80.3</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>635.78458448405718</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="D29" s="1">
+        <v>69.8</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>883.98373983739839</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>1.6619999999999999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>60</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>1239.7783103654883</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>2.0920000000000001</v>
+      </c>
+      <c r="D31" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>1791.2929848693261</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>3.089</v>
+      </c>
+      <c r="D32" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>4024.9136577708005</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>4.008</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>10060.403225806453</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>4.3410000000000002</v>
+      </c>
+      <c r="D34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>16420</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>100</v>
-      </c>
-      <c r="C13" s="1">
-        <v>374</v>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>16402.261001517454</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>4.5949999999999998</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>28250.740740740723</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>4.7510000000000003</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-20.3</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>47510.000000000073</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>4.9269999999999996</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>168057.94520547852</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>4.9660000000000002</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-48</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>363686.47058823734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>